<commit_message>
Change variable name in obs files
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/FAR/Observed/AGR ESW W23-01.xlsx
+++ b/Tests/Validation/Wheat/FAR/Observed/AGR ESW W23-01.xlsx
@@ -20,221 +20,221 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="71">
-  <si>
-    <t>SimulationName</t>
-  </si>
-  <si>
-    <t>Clock.Today</t>
-  </si>
-  <si>
-    <t>Plot</t>
-  </si>
-  <si>
-    <t>Rep</t>
-  </si>
-  <si>
-    <t>Wheat.Phenology.CurrentStageName</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-  </si>
-  <si>
-    <t>TOS</t>
-  </si>
-  <si>
-    <t>Crop</t>
-  </si>
-  <si>
-    <t>Wheat.SowingData.Cultivar</t>
-  </si>
-  <si>
-    <t>Wheat.Phenology.Zadok.Stage</t>
-  </si>
-  <si>
-    <t>Wheat.Phenology.Zadok.Stage.err</t>
-  </si>
-  <si>
-    <t>NDVIModel.Script.NDVI</t>
-  </si>
-  <si>
-    <t>NDVIModel.Script.NDVI.err</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Density</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Density.err</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Moisture</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Moisture.err</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Protein</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Protein.err</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Screenings</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Screenings.err</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Wt</t>
-  </si>
-  <si>
-    <t>Wheat.Grain.Wt.err</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Wheat</t>
-  </si>
-  <si>
-    <t>Waugh</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvWaugh</t>
-  </si>
-  <si>
-    <t>Anapurna</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvAnapurna</t>
-  </si>
-  <si>
-    <t>Accroc</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvAccroc</t>
-  </si>
-  <si>
-    <t>Illabo</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvIllabo</t>
-  </si>
-  <si>
-    <t>Mowhawk</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvMowhawk</t>
-  </si>
-  <si>
-    <t>Longsword</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvLongsword</t>
-  </si>
-  <si>
-    <t>Stockade</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvStockade</t>
-  </si>
-  <si>
-    <t>Nighthawk</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvNighthawk</t>
-  </si>
-  <si>
-    <t>Raider</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvRaider</t>
-  </si>
-  <si>
-    <t>Rockstar</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvRockstar</t>
-  </si>
-  <si>
-    <t>Lancer</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvLancer</t>
-  </si>
-  <si>
-    <t>Scepter</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvScepter</t>
-  </si>
-  <si>
-    <t>Sunmaster</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvSunmaster</t>
-  </si>
-  <si>
-    <t>Vixen</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS1CvVixen</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvWaugh</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvAnapurna</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvAccroc</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvIllabo</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvMowhawk</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvLongsword</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvStockade</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvNighthawk</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvRaider</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvRockstar</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvLancer</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvScepter</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvSunmaster</t>
-  </si>
-  <si>
-    <t>AGR ESW W23-01TOS2CvVixen</t>
-  </si>
-  <si>
-    <t>HarvestRipe</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="71">
+  <x:si>
+    <x:t>SimulationName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Clock.Today</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Plot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rep</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Phenology.CurrentStageName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Experiment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TOS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crop</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.SowingData.Cultivar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Phenology.Zadok.Stage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Phenology.Zadok.Stage.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spectral.NDVI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spectral.NDVI.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Density</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Density.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Moisture</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Moisture.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Protein</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Protein.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Screenings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Screenings.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Wt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat.Grain.Wt.err</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wheat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Waugh</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvWaugh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anapurna</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvAnapurna</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Accroc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvAccroc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Illabo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvIllabo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mowhawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvMowhawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Longsword</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvLongsword</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stockade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvStockade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nighthawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvNighthawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvRaider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rockstar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvRockstar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lancer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvLancer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Scepter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvScepter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sunmaster</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvSunmaster</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vixen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS1CvVixen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvWaugh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvAnapurna</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvAccroc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvIllabo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvMowhawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvLongsword</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvStockade</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvNighthawk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvRaider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvRockstar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvLancer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvScepter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvSunmaster</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AGR ESW W23-01TOS2CvVixen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HarvestRipe</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>